<commit_message>
FEAT #12510 TIME 0:10 update default template
</commit_message>
<xml_diff>
--- a/modules/templates/templates/styles/spreadsheet.xlsx
+++ b/modules/templates/templates/styles/spreadsheet.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="112">
   <si>
     <t xml:space="preserve">TITLE</t>
   </si>
@@ -39,214 +39,367 @@
     <t xml:space="preserve">contact.postal_address</t>
   </si>
   <si>
-    <t xml:space="preserve">[contact.postal_address]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact externe : Type de contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact.contact_type_label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[contact.contact_type_label]</t>
+    <t xml:space="preserve">[recipient.postal_address]</t>
   </si>
   <si>
     <t xml:space="preserve">Contact externe : Structure</t>
   </si>
   <si>
-    <t xml:space="preserve">contact.society</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[contact.society]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact externe : Sigle de la structure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact.society_short</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[contact.society_short]</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">recipient.company]</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Contact externes : nom du contact</t>
   </si>
   <si>
-    <t xml:space="preserve">contact.contact_lastname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[contact.contact_lastname]</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">recipient.lastname]</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Contact externes : prénom du contact</t>
   </si>
   <si>
-    <t xml:space="preserve">contact.contact_firstname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[contact.contact_firstname]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact externe : Adresse Dénomination</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact.contact_purpose_label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[contact.contact_purpose_label]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact externe : Adresse Service</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact.departement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[contact.departement]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact externe : Adresse Civilité</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact.title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[contact.title]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact externe : Adresse Nom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact.lastname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[contact.lastname]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact externe : Adresse Prénom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact.firstname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[contact.firstname]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact externe : Adresse Fonction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact.function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[contact.function]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact externe : Adresse Etage, bureau, porte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact.occupancy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[contact.occupancy]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact externe : Adresse N°</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact.address_num</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[contact.address_num]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact externe : Adresse Rue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact.address_street</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[contact.address_street]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact externe : Adresse Complément</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact.address_complement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[contact.address_complement]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact externe : Adresse Code Postal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact.address_postal_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[contact.address_postal_code]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact externe : Adresse Ville</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact.address_town</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[contact.address_town]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact externe : Adresse Pays</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact.address_country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[contact.address_country]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact externe : Adresse Téléphone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact.phone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[contact.phone]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact externe : Adresse Courriel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact.email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[contact.email]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact externe : Adresse Site internet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact.website</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[contact.website]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact externe : Formule de politesse de début de courrier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact.salutation_header</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[contact.salutation_header]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact externe : Formule de politesse de fin de courrier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact.salutation_footer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[contact.salutation_footer]</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">recipient.firstname]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe :  Service</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">recipient.departement]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe :  Civilité</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">recipient.civility]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe :  Fonction</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">recipient.function]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe :  Etage, bureau, porte</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">recipient.address_additional1]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe :  N°</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">recipient.address_number]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe :  Rue</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">recipient.address_street]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe :  Complément</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">recipient.address_additional2]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe :  Code Postal</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">recipient.address_postcode]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe :  Ville</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">recipient.address_town]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe :  Pays</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">recipient.address_country]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe :  Téléphone</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">recipient.phone]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe :  Courriel</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">recipient.email]</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Contact interne: Nom</t>
@@ -378,10 +531,10 @@
     <t xml:space="preserve">Réponse : Numéro chrono de la réponse</t>
   </si>
   <si>
-    <t xml:space="preserve">attachments.chrono</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[attachments.chrono]</t>
+    <t xml:space="preserve">attachment.chrono</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[attachment.chrono]</t>
   </si>
   <si>
     <t xml:space="preserve">Document: Auteur</t>
@@ -484,7 +637,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -514,6 +667,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -564,7 +723,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -574,6 +733,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -658,10 +821,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C13:C14"/>
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -696,560 +859,433 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="0" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="0" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="C8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="0" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="C10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="0" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="C11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="0" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C12" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="C13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="0" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="C14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="0" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C15" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="C16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="0" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="C17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="0" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C18" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>59</v>
-      </c>
-    </row>
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>115</v>
+        <v>37</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>116</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>118</v>
+        <v>40</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>119</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>128</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>133</v>
+      <c r="A46" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="B47" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>136</v>
+      <c r="A47" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="B49" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>138</v>
+      <c r="A49" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
+      <c r="A51" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1269,7 +1305,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C13:C14 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1295,7 +1331,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C13:C14 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
FIX #12091 TIME 0:25 update template with [attachmentRecipient. intead of [recipient.
</commit_message>
<xml_diff>
--- a/modules/templates/templates/styles/spreadsheet.xlsx
+++ b/modules/templates/templates/styles/spreadsheet.xlsx
@@ -39,367 +39,97 @@
     <t xml:space="preserve">contact.postal_address</t>
   </si>
   <si>
-    <t xml:space="preserve">[recipient.postal_address]</t>
+    <t xml:space="preserve">[attachmentRecipient.postal_address]</t>
   </si>
   <si>
     <t xml:space="preserve">Contact externe : Structure</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">recipient.company]</t>
-    </r>
+    <t xml:space="preserve">[attachmentRecipient.company]</t>
   </si>
   <si>
     <t xml:space="preserve">Contact externes : nom du contact</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">recipient.lastname]</t>
-    </r>
+    <t xml:space="preserve">[attachmentRecipient.lastname]</t>
   </si>
   <si>
     <t xml:space="preserve">Contact externes : prénom du contact</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">recipient.firstname]</t>
-    </r>
+    <t xml:space="preserve">[attachmentRecipient.firstname]</t>
   </si>
   <si>
     <t xml:space="preserve">Contact externe :  Service</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">recipient.departement]</t>
-    </r>
+    <t xml:space="preserve">[attachmentRecipient.departement]</t>
   </si>
   <si>
     <t xml:space="preserve">Contact externe :  Civilité</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">recipient.civility]</t>
-    </r>
+    <t xml:space="preserve">[attachmentRecipient.civility]</t>
   </si>
   <si>
     <t xml:space="preserve">Contact externe :  Fonction</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">recipient.function]</t>
-    </r>
+    <t xml:space="preserve">[attachmentRecipient.function]</t>
   </si>
   <si>
     <t xml:space="preserve">Contact externe :  Etage, bureau, porte</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">recipient.address_additional1]</t>
-    </r>
+    <t xml:space="preserve">[attachmentRecipient.address_additional1]</t>
   </si>
   <si>
     <t xml:space="preserve">Contact externe :  N°</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">recipient.address_number]</t>
-    </r>
+    <t xml:space="preserve">[attachmentRecipient.address_number]</t>
   </si>
   <si>
     <t xml:space="preserve">Contact externe :  Rue</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">recipient.address_street]</t>
-    </r>
+    <t xml:space="preserve">[attachmentRecipient.address_street]</t>
   </si>
   <si>
     <t xml:space="preserve">Contact externe :  Complément</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">recipient.address_additional2]</t>
-    </r>
+    <t xml:space="preserve">[attachmentRecipient.address_additional2]</t>
   </si>
   <si>
     <t xml:space="preserve">Contact externe :  Code Postal</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">recipient.address_postcode]</t>
-    </r>
+    <t xml:space="preserve">[attachmentRecipient.address_postcode]</t>
   </si>
   <si>
     <t xml:space="preserve">Contact externe :  Ville</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">recipient.address_town]</t>
-    </r>
+    <t xml:space="preserve">[attachmentRecipient.address_town]</t>
   </si>
   <si>
     <t xml:space="preserve">Contact externe :  Pays</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">recipient.address_country]</t>
-    </r>
+    <t xml:space="preserve">[attachmentRecipient.address_country]</t>
   </si>
   <si>
     <t xml:space="preserve">Contact externe :  Téléphone</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">recipient.phone]</t>
-    </r>
+    <t xml:space="preserve">[attachmentRecipient.phone]</t>
   </si>
   <si>
     <t xml:space="preserve">Contact externe :  Courriel</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">recipient.email]</t>
-    </r>
+    <t xml:space="preserve">[attachmentRecipient.email]</t>
   </si>
   <si>
     <t xml:space="preserve">Contact interne: Nom</t>
@@ -637,7 +367,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -667,12 +397,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -723,7 +447,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -733,10 +457,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -824,7 +544,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -863,7 +583,7 @@
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -871,7 +591,7 @@
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -879,7 +599,7 @@
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -887,7 +607,7 @@
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -895,7 +615,7 @@
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -903,7 +623,7 @@
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -911,7 +631,7 @@
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -919,7 +639,7 @@
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -927,7 +647,7 @@
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -935,7 +655,7 @@
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -943,7 +663,7 @@
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -951,7 +671,7 @@
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -959,7 +679,7 @@
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -967,7 +687,7 @@
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -975,7 +695,7 @@
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1234,50 +954,50 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="3" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="3" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="3" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>